<commit_message>
update frontend for excel update
</commit_message>
<xml_diff>
--- a/Excel/trip_1.xlsx
+++ b/Excel/trip_1.xlsx
@@ -3679,7 +3679,7 @@
       </c>
       <c r="E40" s="112">
         <f aca="false">IF(M4="Y",SUM(E36:E39,'Page 2'!E40,'Page 3'!E40),SUM(E36:E39))</f>
-        <v>192.0</v>
+        <v>0.0</v>
       </c>
       <c r="F40" s="113"/>
       <c r="G40" s="73"/>
@@ -3692,7 +3692,7 @@
       <c r="L40" s="115"/>
       <c r="M40" s="116">
         <f aca="false">IF(M4="Y",SUM(M36:M39,I36:I40,'Page 2'!M40,'Page 3'!M40),SUM(M36:M39,I36:I40))</f>
-        <v>123.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="41" spans="1:13" customFormat="false" ht="15.75" hidden="false" customHeight="1" outlineLevel="0" collapsed="false">

</xml_diff>